<commit_message>
Latest Data Update - 12months
Latest Data Update - 12 months completed but requires reviewing entries
before submitting for QA
</commit_message>
<xml_diff>
--- a/eng/SOTD_QuestionAudit.xlsx
+++ b/eng/SOTD_QuestionAudit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="1655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1663">
   <si>
     <t>Question Number</t>
   </si>
@@ -5785,6 +5785,30 @@
   </si>
   <si>
     <t>03-22-YYYY</t>
+  </si>
+  <si>
+    <t>03-23-YYYY</t>
+  </si>
+  <si>
+    <t>03-24-YYYY</t>
+  </si>
+  <si>
+    <t>03-25-YYYY</t>
+  </si>
+  <si>
+    <t>03-26-YYYY</t>
+  </si>
+  <si>
+    <t>03-27-YYYY</t>
+  </si>
+  <si>
+    <t>03-28-YYYY</t>
+  </si>
+  <si>
+    <t>03-29-YYYY</t>
+  </si>
+  <si>
+    <t>03-30-YYYY</t>
   </si>
 </sst>
 </file>
@@ -6872,8 +6896,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H210" sqref="H210"/>
+      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F368" sqref="F368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14024,6 +14048,9 @@
       <c r="E360" s="20" t="s">
         <v>576</v>
       </c>
+      <c r="F360" s="62" t="s">
+        <v>1655</v>
+      </c>
     </row>
     <row r="361" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A361" s="10">
@@ -14041,7 +14068,9 @@
       <c r="E361" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="F361" s="63"/>
+      <c r="F361" s="63" t="s">
+        <v>1656</v>
+      </c>
     </row>
     <row r="362" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
@@ -14059,6 +14088,9 @@
       <c r="E362" s="19" t="s">
         <v>581</v>
       </c>
+      <c r="F362" s="62" t="s">
+        <v>1657</v>
+      </c>
     </row>
     <row r="363" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A363" s="10">
@@ -14076,7 +14108,9 @@
       <c r="E363" s="18" t="s">
         <v>625</v>
       </c>
-      <c r="F363" s="63"/>
+      <c r="F363" s="63" t="s">
+        <v>1658</v>
+      </c>
     </row>
     <row r="364" spans="1:6" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A364" s="10">
@@ -14094,7 +14128,9 @@
       <c r="E364" s="18" t="s">
         <v>627</v>
       </c>
-      <c r="F364" s="63"/>
+      <c r="F364" s="63" t="s">
+        <v>1659</v>
+      </c>
     </row>
     <row r="365" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A365" s="10">
@@ -14112,7 +14148,9 @@
       <c r="E365" s="18" t="s">
         <v>585</v>
       </c>
-      <c r="F365" s="64"/>
+      <c r="F365" s="64" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="366" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A366" s="10">
@@ -14130,7 +14168,9 @@
       <c r="E366" s="18" t="s">
         <v>586</v>
       </c>
-      <c r="F366" s="63"/>
+      <c r="F366" s="63" t="s">
+        <v>1661</v>
+      </c>
     </row>
     <row r="367" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A367" s="7">
@@ -14164,7 +14204,9 @@
       <c r="E368" s="18" t="s">
         <v>591</v>
       </c>
-      <c r="F368" s="63"/>
+      <c r="F368" s="63" t="s">
+        <v>1662</v>
+      </c>
     </row>
     <row r="369" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A369" s="10">

</xml_diff>

<commit_message>
Latest Data check and Re-do - done april
Latest Data check and Re-do - done april which was the worst because of
changes
</commit_message>
<xml_diff>
--- a/eng/SOTD_QuestionAudit.xlsx
+++ b/eng/SOTD_QuestionAudit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1664">
   <si>
     <t>Question Number</t>
   </si>
@@ -4800,9 +4800,6 @@
     <t>04-30-YYYY</t>
   </si>
   <si>
-    <t>04-31-YYYY</t>
-  </si>
-  <si>
     <t>05-01-YYYY</t>
   </si>
   <si>
@@ -5809,6 +5806,12 @@
   </si>
   <si>
     <t>03-30-YYYY</t>
+  </si>
+  <si>
+    <t>04-02-YYYY</t>
+  </si>
+  <si>
+    <t>04-01-YYYY</t>
   </si>
 </sst>
 </file>
@@ -6896,8 +6899,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F368" sqref="F368"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7158,7 +7161,7 @@
         <v>714</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>984</v>
@@ -7506,9 +7509,7 @@
       <c r="E30" s="19" t="s">
         <v>638</v>
       </c>
-      <c r="F30" s="65" t="s">
-        <v>1327</v>
-      </c>
+      <c r="F30" s="65"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
@@ -7544,7 +7545,7 @@
         <v>641</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7564,7 +7565,7 @@
         <v>644</v>
       </c>
       <c r="F33" s="63" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7584,7 +7585,7 @@
         <v>646</v>
       </c>
       <c r="F34" s="62" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7604,7 +7605,7 @@
         <v>649</v>
       </c>
       <c r="F35" s="62" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -7624,7 +7625,7 @@
         <v>651</v>
       </c>
       <c r="F36" s="62" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7644,7 +7645,7 @@
         <v>654</v>
       </c>
       <c r="F37" s="63" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7664,7 +7665,7 @@
         <v>682</v>
       </c>
       <c r="F38" s="62" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7684,7 +7685,7 @@
         <v>667</v>
       </c>
       <c r="F39" s="62" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -7704,7 +7705,7 @@
         <v>668</v>
       </c>
       <c r="F40" s="62" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -7724,7 +7725,7 @@
         <v>671</v>
       </c>
       <c r="F41" s="63" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7744,7 +7745,7 @@
         <v>674</v>
       </c>
       <c r="F42" s="62" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7764,7 +7765,7 @@
         <v>675</v>
       </c>
       <c r="F43" s="62" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7784,7 +7785,7 @@
         <v>679</v>
       </c>
       <c r="F44" s="63" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7804,7 +7805,7 @@
         <v>726</v>
       </c>
       <c r="F45" s="63" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="12" customFormat="1" ht="150" x14ac:dyDescent="0.25">
@@ -7824,7 +7825,7 @@
         <v>734</v>
       </c>
       <c r="F46" s="63" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7844,7 +7845,7 @@
         <v>72</v>
       </c>
       <c r="F47" s="64" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7882,7 +7883,7 @@
         <v>88</v>
       </c>
       <c r="F49" s="62" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7902,7 +7903,7 @@
         <v>91</v>
       </c>
       <c r="F50" s="62" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7922,7 +7923,7 @@
         <v>94</v>
       </c>
       <c r="F51" s="62" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -7942,7 +7943,7 @@
         <v>96</v>
       </c>
       <c r="F52" s="62" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7962,7 +7963,7 @@
         <v>99</v>
       </c>
       <c r="F53" s="63" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7982,7 +7983,7 @@
         <v>78</v>
       </c>
       <c r="F54" s="63" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8002,7 +8003,7 @@
         <v>80</v>
       </c>
       <c r="F55" s="63" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -8022,7 +8023,7 @@
         <v>102</v>
       </c>
       <c r="F56" s="62" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8042,7 +8043,7 @@
         <v>83</v>
       </c>
       <c r="F57" s="62" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8062,7 +8063,7 @@
         <v>86</v>
       </c>
       <c r="F58" s="63" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8082,7 +8083,7 @@
         <v>104</v>
       </c>
       <c r="F59" s="62" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="59" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8093,7 +8094,7 @@
         <v>106</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D60" s="57" t="s">
         <v>1086</v>
@@ -8102,7 +8103,7 @@
         <v>105</v>
       </c>
       <c r="F60" s="62" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -8122,7 +8123,7 @@
         <v>109</v>
       </c>
       <c r="F61" s="62" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8142,7 +8143,7 @@
         <v>111</v>
       </c>
       <c r="F62" s="63" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8162,7 +8163,7 @@
         <v>737</v>
       </c>
       <c r="F63" s="62" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8182,7 +8183,7 @@
         <v>114</v>
       </c>
       <c r="F64" s="63" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -8202,7 +8203,7 @@
         <v>157</v>
       </c>
       <c r="F65" s="62" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -8222,7 +8223,7 @@
         <v>158</v>
       </c>
       <c r="F66" s="62" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -8242,7 +8243,7 @@
         <v>159</v>
       </c>
       <c r="F67" s="62" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -8262,7 +8263,7 @@
         <v>163</v>
       </c>
       <c r="F68" s="62" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -8282,7 +8283,7 @@
         <v>165</v>
       </c>
       <c r="F69" s="62" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8302,7 +8303,7 @@
         <v>141</v>
       </c>
       <c r="F70" s="63" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8322,7 +8323,7 @@
         <v>117</v>
       </c>
       <c r="F71" s="63" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8342,7 +8343,7 @@
         <v>122</v>
       </c>
       <c r="F72" s="63" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8362,7 +8363,7 @@
         <v>125</v>
       </c>
       <c r="F73" s="63" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -8382,7 +8383,7 @@
         <v>127</v>
       </c>
       <c r="F74" s="62" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8402,7 +8403,7 @@
         <v>130</v>
       </c>
       <c r="F75" s="62" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8422,7 +8423,7 @@
         <v>133</v>
       </c>
       <c r="F76" s="63" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8442,7 +8443,7 @@
         <v>134</v>
       </c>
       <c r="F77" s="63" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8462,7 +8463,7 @@
         <v>137</v>
       </c>
       <c r="F78" s="63" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8482,7 +8483,7 @@
         <v>142</v>
       </c>
       <c r="F79" s="63" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8502,7 +8503,7 @@
         <v>145</v>
       </c>
       <c r="F80" s="63" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8522,7 +8523,7 @@
         <v>146</v>
       </c>
       <c r="F81" s="62" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8542,7 +8543,7 @@
         <v>148</v>
       </c>
       <c r="F82" s="62" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8562,7 +8563,7 @@
         <v>152</v>
       </c>
       <c r="F83" s="62" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8582,7 +8583,7 @@
         <v>741</v>
       </c>
       <c r="F84" s="63" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8602,7 +8603,7 @@
         <v>175</v>
       </c>
       <c r="F85" s="62" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -8622,7 +8623,7 @@
         <v>178</v>
       </c>
       <c r="F86" s="62" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -8642,7 +8643,7 @@
         <v>180</v>
       </c>
       <c r="F87" s="62" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -8662,7 +8663,7 @@
         <v>166</v>
       </c>
       <c r="F88" s="62" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8682,7 +8683,7 @@
         <v>168</v>
       </c>
       <c r="F89" s="62" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8702,7 +8703,7 @@
         <v>174</v>
       </c>
       <c r="F90" s="63" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8722,7 +8723,7 @@
         <v>199</v>
       </c>
       <c r="F91" s="63" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8742,7 +8743,7 @@
         <v>202</v>
       </c>
       <c r="F92" s="62" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -8762,7 +8763,7 @@
         <v>203</v>
       </c>
       <c r="F93" s="62" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8782,7 +8783,7 @@
         <v>207</v>
       </c>
       <c r="F94" s="63" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8802,7 +8803,7 @@
         <v>209</v>
       </c>
       <c r="F95" s="62" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8822,7 +8823,7 @@
         <v>184</v>
       </c>
       <c r="F96" s="62" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="97" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8842,7 +8843,7 @@
         <v>212</v>
       </c>
       <c r="F97" s="63" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -8862,7 +8863,7 @@
         <v>187</v>
       </c>
       <c r="F98" s="63" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -8882,7 +8883,7 @@
         <v>190</v>
       </c>
       <c r="F99" s="62" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="100" spans="1:6" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8920,7 +8921,7 @@
         <v>196</v>
       </c>
       <c r="F101" s="66" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
@@ -8940,7 +8941,7 @@
         <v>213</v>
       </c>
       <c r="F102" s="66" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -8960,7 +8961,7 @@
         <v>216</v>
       </c>
       <c r="F103" s="62" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -8980,7 +8981,7 @@
         <v>217</v>
       </c>
       <c r="F104" s="62" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9000,7 +9001,7 @@
         <v>219</v>
       </c>
       <c r="F105" s="62" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -9020,7 +9021,7 @@
         <v>220</v>
       </c>
       <c r="F106" s="62" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9040,7 +9041,7 @@
         <v>221</v>
       </c>
       <c r="F107" s="62" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -9060,7 +9061,7 @@
         <v>224</v>
       </c>
       <c r="F108" s="62" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9080,7 +9081,7 @@
         <v>226</v>
       </c>
       <c r="F109" s="62" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9100,7 +9101,7 @@
         <v>229</v>
       </c>
       <c r="F110" s="62" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -9120,7 +9121,7 @@
         <v>254</v>
       </c>
       <c r="F111" s="63" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9140,7 +9141,7 @@
         <v>256</v>
       </c>
       <c r="F112" s="62" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -9160,7 +9161,7 @@
         <v>258</v>
       </c>
       <c r="F113" s="62" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -9180,7 +9181,7 @@
         <v>232</v>
       </c>
       <c r="F114" s="63" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="115" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9200,7 +9201,7 @@
         <v>235</v>
       </c>
       <c r="F115" s="63" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -9220,7 +9221,7 @@
         <v>236</v>
       </c>
       <c r="F116" s="63" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -9240,7 +9241,7 @@
         <v>241</v>
       </c>
       <c r="F117" s="62" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9260,7 +9261,7 @@
         <v>242</v>
       </c>
       <c r="F118" s="62" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9280,7 +9281,7 @@
         <v>243</v>
       </c>
       <c r="F119" s="62" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9300,7 +9301,7 @@
         <v>244</v>
       </c>
       <c r="F120" s="63" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9320,7 +9321,7 @@
         <v>252</v>
       </c>
       <c r="F121" s="62" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -9340,7 +9341,7 @@
         <v>259</v>
       </c>
       <c r="F122" s="62" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9360,7 +9361,7 @@
         <v>260</v>
       </c>
       <c r="F123" s="62" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="124" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -9380,7 +9381,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="63" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9400,7 +9401,7 @@
         <v>268</v>
       </c>
       <c r="F125" s="62" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -9420,7 +9421,7 @@
         <v>24</v>
       </c>
       <c r="F126" s="64" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9440,7 +9441,7 @@
         <v>25</v>
       </c>
       <c r="F127" s="63" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -9448,7 +9449,7 @@
         <v>3</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>6</v>
@@ -9460,7 +9461,7 @@
         <v>26</v>
       </c>
       <c r="F128" s="62" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9480,7 +9481,7 @@
         <v>27</v>
       </c>
       <c r="F129" s="62" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9500,7 +9501,7 @@
         <v>28</v>
       </c>
       <c r="F130" s="62" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -9520,7 +9521,7 @@
         <v>29</v>
       </c>
       <c r="F131" s="62" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9540,7 +9541,7 @@
         <v>30</v>
       </c>
       <c r="F132" s="62" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9560,7 +9561,7 @@
         <v>31</v>
       </c>
       <c r="F133" s="62" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -9580,7 +9581,7 @@
         <v>32</v>
       </c>
       <c r="F134" s="62" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9600,7 +9601,7 @@
         <v>33</v>
       </c>
       <c r="F135" s="62" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="136" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9620,7 +9621,7 @@
         <v>34</v>
       </c>
       <c r="F136" s="63" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -9640,7 +9641,7 @@
         <v>37</v>
       </c>
       <c r="F137" s="62" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -9660,7 +9661,7 @@
         <v>39</v>
       </c>
       <c r="F138" s="62" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -9680,7 +9681,7 @@
         <v>42</v>
       </c>
       <c r="F139" s="62" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -9700,7 +9701,7 @@
         <v>43</v>
       </c>
       <c r="F140" s="62" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="141" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -9720,7 +9721,7 @@
         <v>47</v>
       </c>
       <c r="F141" s="62" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="142" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9740,7 +9741,7 @@
         <v>49</v>
       </c>
       <c r="F142" s="63" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="143" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -9760,7 +9761,7 @@
         <v>52</v>
       </c>
       <c r="F143" s="63" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -9780,7 +9781,7 @@
         <v>55</v>
       </c>
       <c r="F144" s="62" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="32.25" x14ac:dyDescent="0.25">
@@ -9800,7 +9801,7 @@
         <v>58</v>
       </c>
       <c r="F145" s="62" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -9820,7 +9821,7 @@
         <v>61</v>
       </c>
       <c r="F146" s="62" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -9840,7 +9841,7 @@
         <v>64</v>
       </c>
       <c r="F147" s="62" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9860,7 +9861,7 @@
         <v>744</v>
       </c>
       <c r="F148" s="62" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="149" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -9880,7 +9881,7 @@
         <v>295</v>
       </c>
       <c r="F149" s="63" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="150" spans="1:6" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -9900,7 +9901,7 @@
         <v>297</v>
       </c>
       <c r="F150" s="63" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="151" spans="1:6" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -9920,7 +9921,7 @@
         <v>299</v>
       </c>
       <c r="F151" s="63" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="152" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -9940,7 +9941,7 @@
         <v>270</v>
       </c>
       <c r="F152" s="62" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="153" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9960,7 +9961,7 @@
         <v>273</v>
       </c>
       <c r="F153" s="62" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -9980,7 +9981,7 @@
         <v>275</v>
       </c>
       <c r="F154" s="62" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -10000,7 +10001,7 @@
         <v>277</v>
       </c>
       <c r="F155" s="62" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10020,7 +10021,7 @@
         <v>281</v>
       </c>
       <c r="F156" s="63" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="157" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10040,7 +10041,7 @@
         <v>282</v>
       </c>
       <c r="F157" s="63" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="158" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -10060,7 +10061,7 @@
         <v>286</v>
       </c>
       <c r="F158" s="63" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -10080,7 +10081,7 @@
         <v>289</v>
       </c>
       <c r="F159" s="62" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="160" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -10100,7 +10101,7 @@
         <v>292</v>
       </c>
       <c r="F160" s="63" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -10120,7 +10121,7 @@
         <v>301</v>
       </c>
       <c r="F161" s="62" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10140,7 +10141,7 @@
         <v>303</v>
       </c>
       <c r="F162" s="62" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -10160,7 +10161,7 @@
         <v>305</v>
       </c>
       <c r="F163" s="62" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="164" spans="1:6" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -10180,7 +10181,7 @@
         <v>309</v>
       </c>
       <c r="F164" s="69" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="165" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -10200,7 +10201,7 @@
         <v>310</v>
       </c>
       <c r="F165" s="63" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10220,7 +10221,7 @@
         <v>311</v>
       </c>
       <c r="F166" s="62" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -10240,7 +10241,7 @@
         <v>312</v>
       </c>
       <c r="F167" s="62" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="168" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -10260,7 +10261,7 @@
         <v>314</v>
       </c>
       <c r="F168" s="63" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -10280,7 +10281,7 @@
         <v>315</v>
       </c>
       <c r="F169" s="62" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -10300,7 +10301,7 @@
         <v>316</v>
       </c>
       <c r="F170" s="62" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="171" spans="1:6" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -10320,7 +10321,7 @@
         <v>319</v>
       </c>
       <c r="F171" s="63" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -10340,7 +10341,7 @@
         <v>321</v>
       </c>
       <c r="F172" s="62" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -10360,7 +10361,7 @@
         <v>324</v>
       </c>
       <c r="F173" s="62" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10380,7 +10381,7 @@
         <v>327</v>
       </c>
       <c r="F174" s="62" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10400,7 +10401,7 @@
         <v>341</v>
       </c>
       <c r="F175" s="62" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10420,7 +10421,7 @@
         <v>345</v>
       </c>
       <c r="F176" s="62" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="177" spans="1:6" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -10438,7 +10439,7 @@
         <v>1186</v>
       </c>
       <c r="F177" s="67" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="178" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -10458,7 +10459,7 @@
         <v>332</v>
       </c>
       <c r="F178" s="63" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="179" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -10478,7 +10479,7 @@
         <v>334</v>
       </c>
       <c r="F179" s="63" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10498,7 +10499,7 @@
         <v>336</v>
       </c>
       <c r="F180" s="62" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -10518,7 +10519,7 @@
         <v>337</v>
       </c>
       <c r="F181" s="62" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -10538,7 +10539,7 @@
         <v>340</v>
       </c>
       <c r="F182" s="62" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -10558,7 +10559,7 @@
         <v>347</v>
       </c>
       <c r="F183" s="62" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -10578,7 +10579,7 @@
         <v>350</v>
       </c>
       <c r="F184" s="62" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -10598,7 +10599,7 @@
         <v>352</v>
       </c>
       <c r="F185" s="62" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10618,7 +10619,7 @@
         <v>355</v>
       </c>
       <c r="F186" s="62" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10638,7 +10639,7 @@
         <v>357</v>
       </c>
       <c r="F187" s="62" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -10658,7 +10659,7 @@
         <v>346</v>
       </c>
       <c r="F188" s="62" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -10678,7 +10679,7 @@
         <v>359</v>
       </c>
       <c r="F189" s="62" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -10698,7 +10699,7 @@
         <v>362</v>
       </c>
       <c r="F190" s="62" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -10718,7 +10719,7 @@
         <v>365</v>
       </c>
       <c r="F191" s="62" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -10738,7 +10739,7 @@
         <v>367</v>
       </c>
       <c r="F192" s="62" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -10758,7 +10759,7 @@
         <v>368</v>
       </c>
       <c r="F193" s="62" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -10778,7 +10779,7 @@
         <v>375</v>
       </c>
       <c r="F194" s="62" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="195" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -10798,7 +10799,7 @@
         <v>371</v>
       </c>
       <c r="F195" s="63" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="196" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10818,7 +10819,7 @@
         <v>374</v>
       </c>
       <c r="F196" s="62" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
@@ -10838,7 +10839,7 @@
         <v>387</v>
       </c>
       <c r="F197" s="62" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="198" spans="1:6" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10858,7 +10859,7 @@
         <v>388</v>
       </c>
       <c r="F198" s="68" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="199" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -10878,7 +10879,7 @@
         <v>391</v>
       </c>
       <c r="F199" s="63" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="200" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -10898,7 +10899,7 @@
         <v>392</v>
       </c>
       <c r="F200" s="63" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
@@ -10918,7 +10919,7 @@
         <v>381</v>
       </c>
       <c r="F201" s="62" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -10938,7 +10939,7 @@
         <v>383</v>
       </c>
       <c r="F202" s="62" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="203" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -10956,7 +10957,7 @@
         <v>761</v>
       </c>
       <c r="F203" s="63" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="204" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -10974,7 +10975,7 @@
         <v>762</v>
       </c>
       <c r="F204" s="63" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="205" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -10992,7 +10993,7 @@
         <v>771</v>
       </c>
       <c r="F205" s="63" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11009,7 +11010,7 @@
         <v>763</v>
       </c>
       <c r="F206" s="62" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11026,7 +11027,7 @@
         <v>764</v>
       </c>
       <c r="F207" s="62" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="208" spans="1:6" s="36" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -11044,7 +11045,7 @@
         <v>765</v>
       </c>
       <c r="F208" s="62" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="209" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -11062,7 +11063,7 @@
         <v>766</v>
       </c>
       <c r="F209" s="72" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="210" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -11080,7 +11081,7 @@
         <v>767</v>
       </c>
       <c r="F210" s="72" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="211" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -11098,7 +11099,7 @@
         <v>768</v>
       </c>
       <c r="F211" s="72" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -11115,7 +11116,7 @@
         <v>769</v>
       </c>
       <c r="F212" s="62" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -11132,7 +11133,7 @@
         <v>770</v>
       </c>
       <c r="F213" s="62" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -11152,7 +11153,7 @@
         <v>425</v>
       </c>
       <c r="F214" s="62" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11172,7 +11173,7 @@
         <v>428</v>
       </c>
       <c r="F215" s="62" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11192,7 +11193,7 @@
         <v>397</v>
       </c>
       <c r="F216" s="62" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="217" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -11212,7 +11213,7 @@
         <v>399</v>
       </c>
       <c r="F217" s="62" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="218" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11232,7 +11233,7 @@
         <v>401</v>
       </c>
       <c r="F218" s="62" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="219" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -11252,7 +11253,7 @@
         <v>403</v>
       </c>
       <c r="F219" s="62" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="220" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -11272,7 +11273,7 @@
         <v>405</v>
       </c>
       <c r="F220" s="62" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="221" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -11292,7 +11293,7 @@
         <v>406</v>
       </c>
       <c r="F221" s="63" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="222" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11312,7 +11313,7 @@
         <v>411</v>
       </c>
       <c r="F222" s="63" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -11332,7 +11333,7 @@
         <v>414</v>
       </c>
       <c r="F223" s="62" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="224" spans="1:6" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -11352,7 +11353,7 @@
         <v>417</v>
       </c>
       <c r="F224" s="63" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="225" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -11372,7 +11373,7 @@
         <v>418</v>
       </c>
       <c r="F225" s="62" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -11392,7 +11393,7 @@
         <v>421</v>
       </c>
       <c r="F226" s="62" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="227" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11412,7 +11413,7 @@
         <v>422</v>
       </c>
       <c r="F227" s="63" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -11432,7 +11433,7 @@
         <v>435</v>
       </c>
       <c r="F228" s="62" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -11452,7 +11453,7 @@
         <v>432</v>
       </c>
       <c r="F229" s="62" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="230" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -11472,7 +11473,7 @@
         <v>434</v>
       </c>
       <c r="F230" s="62" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="231" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11492,7 +11493,7 @@
         <v>773</v>
       </c>
       <c r="F231" s="63" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="210" x14ac:dyDescent="0.25">
@@ -11512,7 +11513,7 @@
         <v>849</v>
       </c>
       <c r="F232" s="62" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="233" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -11532,7 +11533,7 @@
         <v>774</v>
       </c>
       <c r="F233" s="63" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11552,7 +11553,7 @@
         <v>775</v>
       </c>
       <c r="F234" s="62" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -11572,7 +11573,7 @@
         <v>776</v>
       </c>
       <c r="F235" s="62" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
@@ -11592,7 +11593,7 @@
         <v>777</v>
       </c>
       <c r="F236" s="62" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -11612,7 +11613,7 @@
         <v>778</v>
       </c>
       <c r="F237" s="62" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11632,7 +11633,7 @@
         <v>772</v>
       </c>
       <c r="F238" s="62" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11652,7 +11653,7 @@
         <v>439</v>
       </c>
       <c r="F239" s="62" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11672,7 +11673,7 @@
         <v>440</v>
       </c>
       <c r="F240" s="62" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11692,7 +11693,7 @@
         <v>445</v>
       </c>
       <c r="F241" s="62" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="242" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11712,7 +11713,7 @@
         <v>447</v>
       </c>
       <c r="F242" s="62" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="243" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11732,7 +11733,7 @@
         <v>449</v>
       </c>
       <c r="F243" s="63" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="244" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -11752,7 +11753,7 @@
         <v>779</v>
       </c>
       <c r="F244" s="63" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="245" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -11772,7 +11773,7 @@
         <v>786</v>
       </c>
       <c r="F245" s="69" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="246" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11792,7 +11793,7 @@
         <v>787</v>
       </c>
       <c r="F246" s="63" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="247" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11812,7 +11813,7 @@
         <v>788</v>
       </c>
       <c r="F247" s="62" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="248" spans="1:6" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -11832,7 +11833,7 @@
         <v>789</v>
       </c>
       <c r="F248" s="63" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="249" spans="1:6" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -11852,7 +11853,7 @@
         <v>780</v>
       </c>
       <c r="F249" s="69" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -11866,7 +11867,7 @@
         <v>781</v>
       </c>
       <c r="F250" s="69" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -11886,7 +11887,7 @@
         <v>790</v>
       </c>
       <c r="F251" s="62" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -11906,7 +11907,7 @@
         <v>782</v>
       </c>
       <c r="F252" s="62" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11926,7 +11927,7 @@
         <v>783</v>
       </c>
       <c r="F253" s="62" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="254" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -11946,7 +11947,7 @@
         <v>784</v>
       </c>
       <c r="F254" s="63" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -11966,7 +11967,7 @@
         <v>785</v>
       </c>
       <c r="F255" s="62" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11986,7 +11987,7 @@
         <v>476</v>
       </c>
       <c r="F256" s="62" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="257" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -12006,7 +12007,7 @@
         <v>477</v>
       </c>
       <c r="F257" s="62" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -12026,7 +12027,7 @@
         <v>480</v>
       </c>
       <c r="F258" s="62" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12046,7 +12047,7 @@
         <v>482</v>
       </c>
       <c r="F259" s="62" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
@@ -12066,7 +12067,7 @@
         <v>483</v>
       </c>
       <c r="F260" s="62" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12086,7 +12087,7 @@
         <v>487</v>
       </c>
       <c r="F261" s="62" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="32.25" x14ac:dyDescent="0.25">
@@ -12106,7 +12107,7 @@
         <v>488</v>
       </c>
       <c r="F262" s="62" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12126,7 +12127,7 @@
         <v>492</v>
       </c>
       <c r="F263" s="62" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="264" spans="1:6" s="12" customFormat="1" ht="62.25" x14ac:dyDescent="0.25">
@@ -12146,7 +12147,7 @@
         <v>453</v>
       </c>
       <c r="F264" s="63" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="265" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12166,7 +12167,7 @@
         <v>457</v>
       </c>
       <c r="F265" s="69" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="266" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12186,7 +12187,7 @@
         <v>458</v>
       </c>
       <c r="F266" s="69" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="267" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -12206,7 +12207,7 @@
         <v>459</v>
       </c>
       <c r="F267" s="62" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="268" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12226,7 +12227,7 @@
         <v>462</v>
       </c>
       <c r="F268" s="62" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="269" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -12246,7 +12247,7 @@
         <v>465</v>
       </c>
       <c r="F269" s="63" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="270" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12266,7 +12267,7 @@
         <v>468</v>
       </c>
       <c r="F270" s="63" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="271" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12286,7 +12287,7 @@
         <v>469</v>
       </c>
       <c r="F271" s="63" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="272" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12306,7 +12307,7 @@
         <v>474</v>
       </c>
       <c r="F272" s="63" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="273" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12326,7 +12327,7 @@
         <v>793</v>
       </c>
       <c r="F273" s="63" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="274" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12343,7 +12344,7 @@
         <v>794</v>
       </c>
       <c r="F274" s="63" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="275" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12363,7 +12364,7 @@
         <v>795</v>
       </c>
       <c r="F275" s="63" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="276" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -12383,7 +12384,7 @@
         <v>796</v>
       </c>
       <c r="F276" s="62" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="277" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -12403,7 +12404,7 @@
         <v>797</v>
       </c>
       <c r="F277" s="62" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="278" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12423,7 +12424,7 @@
         <v>798</v>
       </c>
       <c r="F278" s="63" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="279" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12443,7 +12444,7 @@
         <v>799</v>
       </c>
       <c r="F279" s="63" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="280" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -12463,7 +12464,7 @@
         <v>800</v>
       </c>
       <c r="F280" s="63" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="281" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12481,7 +12482,7 @@
         <v>801</v>
       </c>
       <c r="F281" s="62" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -12501,7 +12502,7 @@
         <v>802</v>
       </c>
       <c r="F282" s="62" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="283" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12521,7 +12522,7 @@
         <v>803</v>
       </c>
       <c r="F283" s="62" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="284" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12541,7 +12542,7 @@
         <v>804</v>
       </c>
       <c r="F284" s="63" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="285" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12561,7 +12562,7 @@
         <v>805</v>
       </c>
       <c r="F285" s="63" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="286" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12581,7 +12582,7 @@
         <v>806</v>
       </c>
       <c r="F286" s="63" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="287" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12601,7 +12602,7 @@
         <v>807</v>
       </c>
       <c r="F287" s="62" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -12617,7 +12618,7 @@
         <v>791</v>
       </c>
       <c r="F288" s="62" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="289" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12637,7 +12638,7 @@
         <v>808</v>
       </c>
       <c r="F289" s="64" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -12657,7 +12658,7 @@
         <v>792</v>
       </c>
       <c r="F290" s="62" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="291" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -12677,7 +12678,7 @@
         <v>493</v>
       </c>
       <c r="F291" s="63" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="292" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12697,7 +12698,7 @@
         <v>503</v>
       </c>
       <c r="F292" s="63" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="293" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -12717,7 +12718,7 @@
         <v>506</v>
       </c>
       <c r="F293" s="63" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12737,7 +12738,7 @@
         <v>508</v>
       </c>
       <c r="F294" s="62" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="295" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -12757,7 +12758,7 @@
         <v>497</v>
       </c>
       <c r="F295" s="69" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12777,7 +12778,7 @@
         <v>499</v>
       </c>
       <c r="F296" s="62" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12797,7 +12798,7 @@
         <v>811</v>
       </c>
       <c r="F297" s="62" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="298" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12817,7 +12818,7 @@
         <v>812</v>
       </c>
       <c r="F298" s="63" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="299" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12837,7 +12838,7 @@
         <v>813</v>
       </c>
       <c r="F299" s="63" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="300" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -12857,7 +12858,7 @@
         <v>814</v>
       </c>
       <c r="F300" s="63" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="301" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12877,7 +12878,7 @@
         <v>815</v>
       </c>
       <c r="F301" s="63" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="302" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -12897,7 +12898,7 @@
         <v>816</v>
       </c>
       <c r="F302" s="63" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="303" spans="1:6" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -12915,7 +12916,7 @@
         <v>817</v>
       </c>
       <c r="F303" s="67" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -12935,7 +12936,7 @@
         <v>818</v>
       </c>
       <c r="F304" s="62" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -12955,7 +12956,7 @@
         <v>819</v>
       </c>
       <c r="F305" s="62" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="306" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -12975,7 +12976,7 @@
         <v>809</v>
       </c>
       <c r="F306" s="63" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -12995,7 +12996,7 @@
         <v>810</v>
       </c>
       <c r="F307" s="62" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
@@ -13015,7 +13016,7 @@
         <v>515</v>
       </c>
       <c r="F308" s="62" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="309" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13035,7 +13036,7 @@
         <v>518</v>
       </c>
       <c r="F309" s="62" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="310" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -13055,7 +13056,7 @@
         <v>520</v>
       </c>
       <c r="F310" s="62" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="311" spans="1:6" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13066,7 +13067,7 @@
         <v>522</v>
       </c>
       <c r="C311" s="51" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="D311" s="34" t="s">
         <v>1249</v>
@@ -13075,7 +13076,7 @@
         <v>521</v>
       </c>
       <c r="F311" s="62" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="312" spans="1:6" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13095,7 +13096,7 @@
         <v>524</v>
       </c>
       <c r="F312" s="62" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="313" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -13115,7 +13116,7 @@
         <v>511</v>
       </c>
       <c r="F313" s="64" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="314" spans="1:6" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -13135,7 +13136,7 @@
         <v>514</v>
       </c>
       <c r="F314" s="63" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
@@ -13155,7 +13156,7 @@
         <v>525</v>
       </c>
       <c r="F315" s="62" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
@@ -13175,7 +13176,7 @@
         <v>526</v>
       </c>
       <c r="F316" s="62" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13195,7 +13196,7 @@
         <v>823</v>
       </c>
       <c r="F317" s="62" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="318" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13215,7 +13216,7 @@
         <v>824</v>
       </c>
       <c r="F318" s="62" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="319" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13235,7 +13236,7 @@
         <v>825</v>
       </c>
       <c r="F319" s="62" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
@@ -13255,7 +13256,7 @@
         <v>928</v>
       </c>
       <c r="F320" s="62" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="321" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13275,7 +13276,7 @@
         <v>929</v>
       </c>
       <c r="F321" s="62" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="322" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13295,7 +13296,7 @@
         <v>934</v>
       </c>
       <c r="F322" s="63" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -13315,7 +13316,7 @@
         <v>936</v>
       </c>
       <c r="F323" s="62" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13335,7 +13336,7 @@
         <v>820</v>
       </c>
       <c r="F324" s="62" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13355,7 +13356,7 @@
         <v>821</v>
       </c>
       <c r="F325" s="63" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="326" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -13375,7 +13376,7 @@
         <v>822</v>
       </c>
       <c r="F326" s="62" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13395,7 +13396,7 @@
         <v>950</v>
       </c>
       <c r="F327" s="62" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="328" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -13415,7 +13416,7 @@
         <v>951</v>
       </c>
       <c r="F328" s="63" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="329" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -13435,7 +13436,7 @@
         <v>956</v>
       </c>
       <c r="F329" s="63" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13455,7 +13456,7 @@
         <v>959</v>
       </c>
       <c r="F330" s="63" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="331" spans="1:6" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -13475,7 +13476,7 @@
         <v>960</v>
       </c>
       <c r="F331" s="63" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -13495,7 +13496,7 @@
         <v>937</v>
       </c>
       <c r="F332" s="62" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -13515,7 +13516,7 @@
         <v>942</v>
       </c>
       <c r="F333" s="63" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13535,7 +13536,7 @@
         <v>945</v>
       </c>
       <c r="F334" s="62" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="335" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13553,7 +13554,7 @@
         <v>946</v>
       </c>
       <c r="F335" s="62" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="336" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -13573,7 +13574,7 @@
         <v>541</v>
       </c>
       <c r="F336" s="62" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="337" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -13593,7 +13594,7 @@
         <v>542</v>
       </c>
       <c r="F337" s="62" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.25">
@@ -13613,7 +13614,7 @@
         <v>544</v>
       </c>
       <c r="F338" s="62" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.25">
@@ -13633,7 +13634,7 @@
         <v>547</v>
       </c>
       <c r="F339" s="62" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="340" spans="1:6" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -13653,7 +13654,7 @@
         <v>529</v>
       </c>
       <c r="F340" s="64" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="341" spans="1:6" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13673,7 +13674,7 @@
         <v>531</v>
       </c>
       <c r="F341" s="63" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="342" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -13693,7 +13694,7 @@
         <v>532</v>
       </c>
       <c r="F342" s="63" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="343" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -13713,7 +13714,7 @@
         <v>534</v>
       </c>
       <c r="F343" s="62" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13733,7 +13734,7 @@
         <v>537</v>
       </c>
       <c r="F344" s="62" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
@@ -13753,7 +13754,7 @@
         <v>548</v>
       </c>
       <c r="F345" s="62" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -13773,7 +13774,7 @@
         <v>969</v>
       </c>
       <c r="F346" s="62" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="347" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -13793,7 +13794,7 @@
         <v>974</v>
       </c>
       <c r="F347" s="62" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="348" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13813,7 +13814,7 @@
         <v>965</v>
       </c>
       <c r="F348" s="69" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="349" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13833,7 +13834,7 @@
         <v>966</v>
       </c>
       <c r="F349" s="63" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="350" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -13853,7 +13854,7 @@
         <v>553</v>
       </c>
       <c r="F350" s="62" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
@@ -13873,7 +13874,7 @@
         <v>572</v>
       </c>
       <c r="F351" s="62" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="352" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -13893,7 +13894,7 @@
         <v>556</v>
       </c>
       <c r="F352" s="64" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="353" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -13913,7 +13914,7 @@
         <v>560</v>
       </c>
       <c r="F353" s="63" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="354" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13931,7 +13932,7 @@
         <v>561</v>
       </c>
       <c r="F354" s="62" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="355" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13951,7 +13952,7 @@
         <v>565</v>
       </c>
       <c r="F355" s="62" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="356" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -13971,7 +13972,7 @@
         <v>567</v>
       </c>
       <c r="F356" s="63" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="357" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -13991,7 +13992,7 @@
         <v>570</v>
       </c>
       <c r="F357" s="62" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.25">
@@ -14011,7 +14012,7 @@
         <v>574</v>
       </c>
       <c r="F358" s="62" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
@@ -14031,7 +14032,7 @@
         <v>579</v>
       </c>
       <c r="F359" s="62" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="360" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -14049,7 +14050,7 @@
         <v>576</v>
       </c>
       <c r="F360" s="62" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="361" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -14069,7 +14070,7 @@
         <v>577</v>
       </c>
       <c r="F361" s="63" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -14089,7 +14090,7 @@
         <v>581</v>
       </c>
       <c r="F362" s="62" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="363" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -14109,7 +14110,7 @@
         <v>625</v>
       </c>
       <c r="F363" s="63" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="364" spans="1:6" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14129,7 +14130,7 @@
         <v>627</v>
       </c>
       <c r="F364" s="63" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="365" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -14149,7 +14150,7 @@
         <v>585</v>
       </c>
       <c r="F365" s="64" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="366" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14169,7 +14170,7 @@
         <v>586</v>
       </c>
       <c r="F366" s="63" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="367" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14205,7 +14206,7 @@
         <v>591</v>
       </c>
       <c r="F368" s="63" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="369" spans="1:6" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -14224,7 +14225,9 @@
       <c r="E369" s="18" t="s">
         <v>594</v>
       </c>
-      <c r="F369" s="64"/>
+      <c r="F369" s="64" t="s">
+        <v>1662</v>
+      </c>
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
@@ -14241,6 +14244,9 @@
       </c>
       <c r="E370" s="19" t="s">
         <v>595</v>
+      </c>
+      <c r="F370" s="62" t="s">
+        <v>1663</v>
       </c>
     </row>
     <row r="371" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest Data Update check and redo - done May/June
Latest Data Update check and redo - done May and June...and most of July
</commit_message>
<xml_diff>
--- a/eng/SOTD_QuestionAudit.xlsx
+++ b/eng/SOTD_QuestionAudit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1666">
   <si>
     <t>Question Number</t>
   </si>
@@ -5812,6 +5812,12 @@
   </si>
   <si>
     <t>04-01-YYYY</t>
+  </si>
+  <si>
+    <t>06-27-YYYY</t>
+  </si>
+  <si>
+    <t>06-29-YYYY</t>
   </si>
 </sst>
 </file>
@@ -6899,8 +6905,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8703,7 +8709,7 @@
         <v>174</v>
       </c>
       <c r="F90" s="63" t="s">
-        <v>1384</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8743,7 +8749,7 @@
         <v>202</v>
       </c>
       <c r="F92" s="62" t="s">
-        <v>1385</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest up date and check up to Dec
Latest up date and check up to Dec
</commit_message>
<xml_diff>
--- a/eng/SOTD_QuestionAudit.xlsx
+++ b/eng/SOTD_QuestionAudit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="1667">
   <si>
     <t>Question Number</t>
   </si>
@@ -5818,6 +5818,9 @@
   </si>
   <si>
     <t>06-29-YYYY</t>
+  </si>
+  <si>
+    <t>08-31-YYYY</t>
   </si>
 </sst>
 </file>
@@ -6905,8 +6908,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
+      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F371" sqref="F371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14270,6 +14273,9 @@
       </c>
       <c r="E371" s="19" t="s">
         <v>599</v>
+      </c>
+      <c r="F371" s="62" t="s">
+        <v>1666</v>
       </c>
     </row>
     <row r="372" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest Data Update and check complete
Latest Data Update and check complete
</commit_message>
<xml_diff>
--- a/eng/SOTD_QuestionAudit.xlsx
+++ b/eng/SOTD_QuestionAudit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-60" windowWidth="16650" windowHeight="12705"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="16650" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="1667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="1668">
   <si>
     <t>Question Number</t>
   </si>
@@ -5821,6 +5821,9 @@
   </si>
   <si>
     <t>08-31-YYYY</t>
+  </si>
+  <si>
+    <t>see below</t>
   </si>
 </sst>
 </file>
@@ -6908,8 +6911,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F371" sqref="F371"/>
+      <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F377" sqref="F377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11876,7 +11879,7 @@
         <v>781</v>
       </c>
       <c r="F250" s="69" t="s">
-        <v>1545</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -12489,9 +12492,6 @@
       <c r="D281" s="23"/>
       <c r="E281" s="24" t="s">
         <v>801</v>
-      </c>
-      <c r="F281" s="62" t="s">
-        <v>1576</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -12626,9 +12626,6 @@
       <c r="E288" s="24" t="s">
         <v>791</v>
       </c>
-      <c r="F288" s="62" t="s">
-        <v>1583</v>
-      </c>
     </row>
     <row r="289" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A289" s="10">
@@ -13940,9 +13937,6 @@
       <c r="E354" s="20" t="s">
         <v>561</v>
       </c>
-      <c r="F354" s="62" t="s">
-        <v>1648</v>
-      </c>
     </row>
     <row r="355" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
@@ -14058,9 +14052,6 @@
       <c r="E360" s="20" t="s">
         <v>576</v>
       </c>
-      <c r="F360" s="62" t="s">
-        <v>1654</v>
-      </c>
     </row>
     <row r="361" spans="1:6" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A361" s="10">
@@ -14294,6 +14285,9 @@
       <c r="E372" s="19" t="s">
         <v>602</v>
       </c>
+      <c r="F372" s="62" t="s">
+        <v>1545</v>
+      </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
@@ -14311,6 +14305,9 @@
       <c r="E373" s="19" t="s">
         <v>610</v>
       </c>
+      <c r="F373" s="62" t="s">
+        <v>1576</v>
+      </c>
     </row>
     <row r="374" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="10">
@@ -14328,7 +14325,9 @@
       <c r="E374" s="18" t="s">
         <v>611</v>
       </c>
-      <c r="F374" s="62"/>
+      <c r="F374" s="62" t="s">
+        <v>1583</v>
+      </c>
     </row>
     <row r="375" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A375" s="10">
@@ -14346,7 +14345,9 @@
       <c r="E375" s="18" t="s">
         <v>605</v>
       </c>
-      <c r="F375" s="64"/>
+      <c r="F375" s="64" t="s">
+        <v>1648</v>
+      </c>
     </row>
     <row r="376" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A376" s="10">
@@ -14381,6 +14382,9 @@
       </c>
       <c r="E377" s="19" t="s">
         <v>614</v>
+      </c>
+      <c r="F377" s="62" t="s">
+        <v>1654</v>
       </c>
     </row>
     <row r="378" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>